<commit_message>
Avance COMFASUB y Mantenimiento Repuesto Critico Corregido
</commit_message>
<xml_diff>
--- a/WebApplication3/wwwroot/Formatos/ComfasubAlistamientoMaterialComfasub.xlsx
+++ b/WebApplication3/wwwroot/Formatos/ComfasubAlistamientoMaterialComfasub.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SIESMAR\siesmar\WebApplication3\wwwroot\Formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7B3FB9-3719-46C0-B68A-3DD725FB4ACC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6FF438-C49F-4D1C-B464-77ABC21172C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7520" xr2:uid="{CEE48BB1-FD34-4BE9-A004-937286016298}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>UNIDAD</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>FM53</t>
+  </si>
+  <si>
+    <t>99.00</t>
+  </si>
+  <si>
+    <t>99.01</t>
+  </si>
+  <si>
+    <t>99.02</t>
+  </si>
+  <si>
+    <t>99.03</t>
   </si>
 </sst>
 </file>
@@ -102,13 +114,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +439,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,8 +494,8 @@
       <c r="F2" s="1">
         <v>666</v>
       </c>
-      <c r="G2" s="1">
-        <v>69</v>
+      <c r="G2" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -504,8 +517,8 @@
       <c r="F3" s="1">
         <v>666</v>
       </c>
-      <c r="G3" s="1">
-        <v>69</v>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -527,8 +540,8 @@
       <c r="F4" s="1">
         <v>666</v>
       </c>
-      <c r="G4" s="1">
-        <v>69</v>
+      <c r="G4" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -550,8 +563,8 @@
       <c r="F5" s="1">
         <v>666</v>
       </c>
-      <c r="G5" s="1">
-        <v>69</v>
+      <c r="G5" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>